<commit_message>
AT: summary table revisions
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/sumtable_countymeans.xlsx
+++ b/results/initial_descriptives/combined/sumtable_countymeans.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>year</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>lccL8_pcnt</t>
+  </si>
+  <si>
+    <t>lccL12_pcnt</t>
+  </si>
+  <si>
+    <t>lccL34_pcnt</t>
+  </si>
+  <si>
+    <t>lccL56_pcnt</t>
+  </si>
+  <si>
+    <t>lccL78_pcnt</t>
   </si>
   <si>
     <t>crop_nr</t>
@@ -115,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H23"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -539,62 +551,166 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>57.224380493164063</v>
+        <v>27.279594421386719</v>
       </c>
       <c r="C17" s="1">
-        <v>94.518028259277344</v>
+        <v>27.233213424682617</v>
       </c>
       <c r="D17" s="1">
-        <v>124.73121643066406</v>
+        <v>27.179462432861328</v>
       </c>
       <c r="E17" s="1">
-        <v>111.63810729980469</v>
+        <v>27.143133163452148</v>
       </c>
       <c r="F17" s="1">
-        <v>66.280105590820313</v>
+        <v>27.043693542480469</v>
       </c>
       <c r="G17" s="1">
-        <v>75.465164184570313</v>
+        <v>27.007862091064453</v>
       </c>
       <c r="H17" s="1">
-        <v>107.39522552490234</v>
+        <v>26.996816635131836</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="1">
+        <v>36.028423309326172</v>
+      </c>
+      <c r="C18" s="1">
+        <v>36.006706237792969</v>
+      </c>
+      <c r="D18" s="1">
+        <v>35.992000579833984</v>
+      </c>
+      <c r="E18" s="1">
+        <v>35.899997711181641</v>
+      </c>
       <c r="F18" s="1">
-        <v>20.544464111328125</v>
+        <v>35.877849578857422</v>
       </c>
       <c r="G18" s="1">
-        <v>19.215654373168945</v>
+        <v>35.835128784179688</v>
       </c>
       <c r="H18" s="1">
-        <v>16.132402420043945</v>
+        <v>35.84136962890625</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="B19" s="1">
+        <v>18.600509643554688</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.624383926391602</v>
+      </c>
+      <c r="D19" s="1">
+        <v>18.643213272094727</v>
+      </c>
       <c r="E19" s="1">
+        <v>18.670459747314453</v>
+      </c>
+      <c r="F19" s="1">
+        <v>18.726682662963867</v>
+      </c>
+      <c r="G19" s="1">
+        <v>18.755411148071289</v>
+      </c>
+      <c r="H19" s="1">
+        <v>18.766611099243164</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>18.091474533081055</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18.135696411132813</v>
+      </c>
+      <c r="D20" s="1">
+        <v>18.185325622558594</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18.286409378051758</v>
+      </c>
+      <c r="F20" s="1">
+        <v>18.351774215698242</v>
+      </c>
+      <c r="G20" s="1">
+        <v>18.40159797668457</v>
+      </c>
+      <c r="H20" s="1">
+        <v>18.39520263671875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>57.224380493164063</v>
+      </c>
+      <c r="C21" s="1">
+        <v>94.518028259277344</v>
+      </c>
+      <c r="D21" s="1">
+        <v>124.73121643066406</v>
+      </c>
+      <c r="E21" s="1">
+        <v>111.63810729980469</v>
+      </c>
+      <c r="F21" s="1">
+        <v>66.280105590820313</v>
+      </c>
+      <c r="G21" s="1">
+        <v>75.465164184570313</v>
+      </c>
+      <c r="H21" s="1">
+        <v>107.39522552490234</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>20.544464111328125</v>
+      </c>
+      <c r="G22" s="1">
+        <v>19.215654373168945</v>
+      </c>
+      <c r="H22" s="1">
+        <v>16.132402420043945</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
         <v>22257.21875</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F23" s="1">
         <v>28130.1640625</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G23" s="1">
         <v>41444.46484375</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H23" s="1">
         <v>43307.26953125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AT: make point panel (2-pointpanel.do); update sum tables to include new CRP data (3-tables.do); make missing observation workbook (4-dataObsStats.do)
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/sumtable_countymeans.xlsx
+++ b/results/initial_descriptives/combined/sumtable_countymeans.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>year</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>lccL78_pcnt</t>
+  </si>
+  <si>
+    <t>CRP_nr</t>
   </si>
   <si>
     <t>crop_nr</t>
@@ -127,7 +130,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -161,25 +164,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>32.332313537597656</v>
+        <v>32.311275482177734</v>
       </c>
       <c r="C2" s="1">
-        <v>31.298788070678711</v>
+        <v>31.278425216674805</v>
       </c>
       <c r="D2" s="1">
-        <v>29.553890228271484</v>
+        <v>29.534662246704102</v>
       </c>
       <c r="E2" s="1">
-        <v>29.083532333374023</v>
+        <v>29.064609527587891</v>
       </c>
       <c r="F2" s="1">
-        <v>28.575283050537109</v>
+        <v>28.556692123413086</v>
       </c>
       <c r="G2" s="1">
-        <v>27.955966949462891</v>
+        <v>27.937778472900391</v>
       </c>
       <c r="H2" s="1">
-        <v>28.168851852416992</v>
+        <v>28.15052604675293</v>
       </c>
     </row>
     <row r="3">
@@ -190,22 +193,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.85870075225830078</v>
+        <v>0.85814207792282104</v>
       </c>
       <c r="D3" s="1">
-        <v>2.1823241710662842</v>
+        <v>2.1809043884277344</v>
       </c>
       <c r="E3" s="1">
-        <v>2.0761411190032959</v>
+        <v>2.0747904777526855</v>
       </c>
       <c r="F3" s="1">
-        <v>1.8803716897964478</v>
+        <v>1.8791482448577881</v>
       </c>
       <c r="G3" s="1">
-        <v>1.9339430332183838</v>
+        <v>1.9326847791671753</v>
       </c>
       <c r="H3" s="1">
-        <v>1.4021095037460327</v>
+        <v>1.4011971950531006</v>
       </c>
     </row>
     <row r="4">
@@ -213,25 +216,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>34.908100128173828</v>
+        <v>34.885387420654297</v>
       </c>
       <c r="C4" s="1">
-        <v>35.098213195800781</v>
+        <v>35.07537841796875</v>
       </c>
       <c r="D4" s="1">
-        <v>35.120071411132813</v>
+        <v>35.097221374511719</v>
       </c>
       <c r="E4" s="1">
-        <v>35.134029388427734</v>
+        <v>35.111167907714844</v>
       </c>
       <c r="F4" s="1">
-        <v>35.237506866455078</v>
+        <v>35.214580535888672</v>
       </c>
       <c r="G4" s="1">
-        <v>35.257175445556641</v>
+        <v>35.234233856201172</v>
       </c>
       <c r="H4" s="1">
-        <v>35.342998504638672</v>
+        <v>35.320003509521484</v>
       </c>
     </row>
     <row r="5">
@@ -239,25 +242,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>11.899901390075684</v>
+        <v>11.892159461975098</v>
       </c>
       <c r="C5" s="1">
-        <v>11.495857238769531</v>
+        <v>11.488377571105957</v>
       </c>
       <c r="D5" s="1">
-        <v>11.330935478210449</v>
+        <v>11.323563575744629</v>
       </c>
       <c r="E5" s="1">
-        <v>10.851533889770508</v>
+        <v>10.844473838806152</v>
       </c>
       <c r="F5" s="1">
-        <v>10.643988609313965</v>
+        <v>10.637063026428223</v>
       </c>
       <c r="G5" s="1">
-        <v>10.681207656860352</v>
+        <v>10.674258232116699</v>
       </c>
       <c r="H5" s="1">
-        <v>10.694736480712891</v>
+        <v>10.687778472900391</v>
       </c>
     </row>
     <row r="6">
@@ -265,25 +268,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>15.54348087310791</v>
+        <v>15.533368110656738</v>
       </c>
       <c r="C6" s="1">
-        <v>15.309108734130859</v>
+        <v>15.299148559570313</v>
       </c>
       <c r="D6" s="1">
-        <v>15.159688949584961</v>
+        <v>15.149826049804688</v>
       </c>
       <c r="E6" s="1">
-        <v>15.129592895507813</v>
+        <v>15.119749069213867</v>
       </c>
       <c r="F6" s="1">
-        <v>15.120001792907715</v>
+        <v>15.110164642333984</v>
       </c>
       <c r="G6" s="1">
-        <v>15.093488693237305</v>
+        <v>15.08366870880127</v>
       </c>
       <c r="H6" s="1">
-        <v>15.042671203613281</v>
+        <v>15.032883644104004</v>
       </c>
     </row>
     <row r="7">
@@ -291,25 +294,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>5.3162064552307129</v>
+        <v>5.3127474784851074</v>
       </c>
       <c r="C7" s="1">
-        <v>5.9393305778503418</v>
+        <v>5.9354662895202637</v>
       </c>
       <c r="D7" s="1">
-        <v>6.6530900001525879</v>
+        <v>6.6487612724304199</v>
       </c>
       <c r="E7" s="1">
-        <v>7.7251725196838379</v>
+        <v>7.7201461791992188</v>
       </c>
       <c r="F7" s="1">
-        <v>8.5428485870361328</v>
+        <v>8.5372905731201172</v>
       </c>
       <c r="G7" s="1">
-        <v>9.0782184600830078</v>
+        <v>9.0723123550415039</v>
       </c>
       <c r="H7" s="1">
-        <v>9.3486337661743164</v>
+        <v>9.3425521850585938</v>
       </c>
     </row>
     <row r="8">
@@ -317,25 +320,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>17.152181625366211</v>
+        <v>17.206083297729492</v>
       </c>
       <c r="C8" s="1">
-        <v>17.736883163452148</v>
+        <v>17.7904052734375</v>
       </c>
       <c r="D8" s="1">
-        <v>18.433132171630859</v>
+        <v>18.486202239990234</v>
       </c>
       <c r="E8" s="1">
-        <v>19.374965667724609</v>
+        <v>19.427421569824219</v>
       </c>
       <c r="F8" s="1">
-        <v>20.148725509643555</v>
+        <v>20.200677871704102</v>
       </c>
       <c r="G8" s="1">
-        <v>20.621425628662109</v>
+        <v>20.673070907592773</v>
       </c>
       <c r="H8" s="1">
-        <v>20.873767852783203</v>
+        <v>20.925247192382813</v>
       </c>
     </row>
     <row r="9">
@@ -343,25 +346,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2.1994905471801758</v>
+        <v>2.1980595588684082</v>
       </c>
       <c r="C9" s="1">
-        <v>2.188544750213623</v>
+        <v>2.1871206760406494</v>
       </c>
       <c r="D9" s="1">
-        <v>2.1767771244049072</v>
+        <v>2.1753609180450439</v>
       </c>
       <c r="E9" s="1">
-        <v>2.1522207260131836</v>
+        <v>2.1508204936981201</v>
       </c>
       <c r="F9" s="1">
-        <v>2.1300144195556641</v>
+        <v>2.1286287307739258</v>
       </c>
       <c r="G9" s="1">
-        <v>2.1135382652282715</v>
+        <v>2.1121630668640137</v>
       </c>
       <c r="H9" s="1">
-        <v>2.104362964630127</v>
+        <v>2.1029939651489258</v>
       </c>
     </row>
     <row r="10">
@@ -369,25 +372,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>21.844184875488281</v>
+        <v>21.829973220825195</v>
       </c>
       <c r="C10" s="1">
-        <v>21.663557052612305</v>
+        <v>21.649463653564453</v>
       </c>
       <c r="D10" s="1">
-        <v>21.462837219238281</v>
+        <v>21.448871612548828</v>
       </c>
       <c r="E10" s="1">
-        <v>21.188833236694336</v>
+        <v>21.175046920776367</v>
       </c>
       <c r="F10" s="1">
-        <v>20.963130950927734</v>
+        <v>20.949491500854492</v>
       </c>
       <c r="G10" s="1">
-        <v>20.812641143798828</v>
+        <v>20.799098968505859</v>
       </c>
       <c r="H10" s="1">
-        <v>20.739887237548828</v>
+        <v>20.726394653320313</v>
       </c>
     </row>
     <row r="11">
@@ -395,25 +398,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>18.798871994018555</v>
+        <v>18.786640167236328</v>
       </c>
       <c r="C11" s="1">
-        <v>18.672138214111328</v>
+        <v>18.659990310668945</v>
       </c>
       <c r="D11" s="1">
-        <v>18.506221771240234</v>
+        <v>18.494180679321289</v>
       </c>
       <c r="E11" s="1">
-        <v>18.278806686401367</v>
+        <v>18.266914367675781</v>
       </c>
       <c r="F11" s="1">
-        <v>18.108024597167969</v>
+        <v>18.096242904663086</v>
       </c>
       <c r="G11" s="1">
-        <v>18.009159088134766</v>
+        <v>17.997442245483398</v>
       </c>
       <c r="H11" s="1">
-        <v>17.952516555786133</v>
+        <v>17.940835952758789</v>
       </c>
     </row>
     <row r="12">
@@ -421,25 +424,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>11.760732650756836</v>
+        <v>11.753081321716309</v>
       </c>
       <c r="C12" s="1">
-        <v>11.671309471130371</v>
+        <v>11.663716316223145</v>
       </c>
       <c r="D12" s="1">
-        <v>11.555923461914063</v>
+        <v>11.548404693603516</v>
       </c>
       <c r="E12" s="1">
-        <v>11.40102481842041</v>
+        <v>11.393607139587402</v>
       </c>
       <c r="F12" s="1">
-        <v>11.273367881774902</v>
+        <v>11.266033172607422</v>
       </c>
       <c r="G12" s="1">
-        <v>11.193347930908203</v>
+        <v>11.186065673828125</v>
       </c>
       <c r="H12" s="1">
-        <v>11.152796745300293</v>
+        <v>11.145540237426758</v>
       </c>
     </row>
     <row r="13">
@@ -447,25 +450,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2.3752191066741943</v>
+        <v>2.373673677444458</v>
       </c>
       <c r="C13" s="1">
-        <v>2.3601162433624268</v>
+        <v>2.3585808277130127</v>
       </c>
       <c r="D13" s="1">
-        <v>2.3400354385375977</v>
+        <v>2.3385131359100342</v>
       </c>
       <c r="E13" s="1">
-        <v>2.3190281391143799</v>
+        <v>2.3175194263458252</v>
       </c>
       <c r="F13" s="1">
-        <v>2.3039166927337646</v>
+        <v>2.3024177551269531</v>
       </c>
       <c r="G13" s="1">
-        <v>2.2924952507019043</v>
+        <v>2.2910037040710449</v>
       </c>
       <c r="H13" s="1">
-        <v>2.2859783172607422</v>
+        <v>2.2844910621643066</v>
       </c>
     </row>
     <row r="14">
@@ -473,25 +476,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>12.51448917388916</v>
+        <v>12.506346702575684</v>
       </c>
       <c r="C14" s="1">
-        <v>12.442048072814941</v>
+        <v>12.433952331542969</v>
       </c>
       <c r="D14" s="1">
-        <v>12.35645866394043</v>
+        <v>12.348419189453125</v>
       </c>
       <c r="E14" s="1">
-        <v>12.235201835632324</v>
+        <v>12.227241516113281</v>
       </c>
       <c r="F14" s="1">
-        <v>12.138643264770508</v>
+        <v>12.130745887756348</v>
       </c>
       <c r="G14" s="1">
-        <v>12.086548805236816</v>
+        <v>12.07868480682373</v>
       </c>
       <c r="H14" s="1">
-        <v>12.054340362548828</v>
+        <v>12.046497344970703</v>
       </c>
     </row>
     <row r="15">
@@ -499,25 +502,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>12.412484169006348</v>
+        <v>12.40440845489502</v>
       </c>
       <c r="C15" s="1">
-        <v>12.334586143493652</v>
+        <v>12.326560974121094</v>
       </c>
       <c r="D15" s="1">
-        <v>12.24983024597168</v>
+        <v>12.241860389709473</v>
       </c>
       <c r="E15" s="1">
-        <v>12.146387100219727</v>
+        <v>12.138484001159668</v>
       </c>
       <c r="F15" s="1">
-        <v>12.036617279052734</v>
+        <v>12.028786659240723</v>
       </c>
       <c r="G15" s="1">
-        <v>11.974529266357422</v>
+        <v>11.966737747192383</v>
       </c>
       <c r="H15" s="1">
-        <v>11.937031745910645</v>
+        <v>11.929265022277832</v>
       </c>
     </row>
     <row r="16">
@@ -525,25 +528,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>0.94234597682952881</v>
+        <v>0.94173288345336914</v>
       </c>
       <c r="C16" s="1">
-        <v>0.93081504106521606</v>
+        <v>0.9302094578742981</v>
       </c>
       <c r="D16" s="1">
-        <v>0.9187847375869751</v>
+        <v>0.91818696260452271</v>
       </c>
       <c r="E16" s="1">
-        <v>0.90353149175643921</v>
+        <v>0.90294367074966431</v>
       </c>
       <c r="F16" s="1">
-        <v>0.89755988121032715</v>
+        <v>0.89697593450546265</v>
       </c>
       <c r="G16" s="1">
-        <v>0.89631485939025879</v>
+        <v>0.89573168754577637</v>
       </c>
       <c r="H16" s="1">
-        <v>0.89931869506835938</v>
+        <v>0.89873361587524414</v>
       </c>
     </row>
     <row r="17">
@@ -551,25 +554,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>24.043676376342773</v>
+        <v>24.028032302856445</v>
       </c>
       <c r="C17" s="1">
-        <v>23.852102279663086</v>
+        <v>23.836584091186523</v>
       </c>
       <c r="D17" s="1">
-        <v>23.639614105224609</v>
+        <v>23.624233245849609</v>
       </c>
       <c r="E17" s="1">
-        <v>23.341053009033203</v>
+        <v>23.32586669921875</v>
       </c>
       <c r="F17" s="1">
-        <v>23.093145370483398</v>
+        <v>23.078119277954102</v>
       </c>
       <c r="G17" s="1">
-        <v>22.926177978515625</v>
+        <v>22.911262512207031</v>
       </c>
       <c r="H17" s="1">
-        <v>22.84425163269043</v>
+        <v>22.829387664794922</v>
       </c>
     </row>
     <row r="18">
@@ -577,25 +580,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>30.559604644775391</v>
+        <v>30.539722442626953</v>
       </c>
       <c r="C18" s="1">
-        <v>30.343448638916016</v>
+        <v>30.323707580566406</v>
       </c>
       <c r="D18" s="1">
-        <v>30.062145233154297</v>
+        <v>30.042585372924805</v>
       </c>
       <c r="E18" s="1">
-        <v>29.679832458496094</v>
+        <v>29.660520553588867</v>
       </c>
       <c r="F18" s="1">
-        <v>29.381391525268555</v>
+        <v>29.362276077270508</v>
       </c>
       <c r="G18" s="1">
-        <v>29.202508926391602</v>
+        <v>29.183507919311523</v>
       </c>
       <c r="H18" s="1">
-        <v>29.105312347412109</v>
+        <v>29.086376190185547</v>
       </c>
     </row>
     <row r="19">
@@ -603,25 +606,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14.889708518981934</v>
+        <v>14.880021095275879</v>
       </c>
       <c r="C19" s="1">
-        <v>14.802164077758789</v>
+        <v>14.792532920837402</v>
       </c>
       <c r="D19" s="1">
-        <v>14.696494102478027</v>
+        <v>14.686932563781738</v>
       </c>
       <c r="E19" s="1">
-        <v>14.554229736328125</v>
+        <v>14.544760704040527</v>
       </c>
       <c r="F19" s="1">
-        <v>14.442560195922852</v>
+        <v>14.433163642883301</v>
       </c>
       <c r="G19" s="1">
-        <v>14.379043579101563</v>
+        <v>14.369688034057617</v>
       </c>
       <c r="H19" s="1">
-        <v>14.34031867980957</v>
+        <v>14.330988883972168</v>
       </c>
     </row>
     <row r="20">
@@ -629,69 +632,75 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>13.354830741882324</v>
+        <v>13.346141815185547</v>
       </c>
       <c r="C20" s="1">
-        <v>13.265400886535645</v>
+        <v>13.256770133972168</v>
       </c>
       <c r="D20" s="1">
-        <v>13.168615341186523</v>
+        <v>13.16004753112793</v>
       </c>
       <c r="E20" s="1">
-        <v>13.049918174743652</v>
+        <v>13.041427612304688</v>
       </c>
       <c r="F20" s="1">
-        <v>12.934177398681641</v>
+        <v>12.925762176513672</v>
       </c>
       <c r="G20" s="1">
-        <v>12.870843887329102</v>
+        <v>12.862469673156738</v>
       </c>
       <c r="H20" s="1">
-        <v>12.836350440979004</v>
+        <v>12.827999114990234</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
-        <v>57.224380493164063</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="1">
-        <v>94.518028259277344</v>
+        <v>50.865180969238281</v>
       </c>
       <c r="D21" s="1">
-        <v>124.73121643066406</v>
+        <v>52.805267333984375</v>
       </c>
       <c r="E21" s="1">
-        <v>111.63810729980469</v>
+        <v>53.657325744628906</v>
       </c>
       <c r="F21" s="1">
-        <v>66.280105590820313</v>
+        <v>55.877994537353516</v>
       </c>
       <c r="G21" s="1">
-        <v>75.465164184570313</v>
+        <v>59.601699829101563</v>
       </c>
       <c r="H21" s="1">
-        <v>107.39522552490234</v>
+        <v>68.188255310058594</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="1">
+        <v>57.224380493164063</v>
+      </c>
+      <c r="C22" s="1">
+        <v>94.518028259277344</v>
+      </c>
+      <c r="D22" s="1">
+        <v>124.73121643066406</v>
+      </c>
+      <c r="E22" s="1">
+        <v>111.63810729980469</v>
+      </c>
       <c r="F22" s="1">
-        <v>20.544464111328125</v>
+        <v>66.280105590820313</v>
       </c>
       <c r="G22" s="1">
-        <v>19.215654373168945</v>
+        <v>75.465164184570313</v>
       </c>
       <c r="H22" s="1">
-        <v>16.132402420043945</v>
+        <v>107.39522552490234</v>
       </c>
     </row>
     <row r="23">
@@ -701,17 +710,35 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1">
-        <v>22257.21875</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>28130.1640625</v>
+        <v>20.555309295654297</v>
       </c>
       <c r="G23" s="1">
-        <v>41444.46484375</v>
+        <v>19.22590446472168</v>
       </c>
       <c r="H23" s="1">
-        <v>43307.26953125</v>
+        <v>16.138092041015625</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1">
+        <v>22334.931640625</v>
+      </c>
+      <c r="F24" s="1">
+        <v>28291.578125</v>
+      </c>
+      <c r="G24" s="1">
+        <v>41637.09375</v>
+      </c>
+      <c r="H24" s="1">
+        <v>43642.6015625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>